<commit_message>
Added reading Excel files in simple mode with Spark Datatypes
</commit_message>
<xml_diff>
--- a/src/it/resources/testsimple.xlsx
+++ b/src/it/resources/testsimple.xlsx
@@ -62,9 +62,6 @@
     <t>stringcolumn</t>
   </si>
   <si>
-    <t>decimalp3sc3</t>
-  </si>
-  <si>
     <t>shortcolumn</t>
   </si>
   <si>
@@ -72,15 +69,17 @@
   </si>
   <si>
     <t>longcolumn</t>
+  </si>
+  <si>
+    <t>decimalp8sc3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="&quot;WAHR&quot;;&quot;WAHR&quot;;&quot;FALSCH&quot;"/>
-    <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
@@ -113,10 +112,10 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Stand." xfId="0" builtinId="0"/>
@@ -396,14 +395,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="14.33203125" customWidth="1"/>
     <col min="3" max="3" width="16.5" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" customWidth="1"/>
     <col min="9" max="9" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -421,185 +419,186 @@
         <v>9</v>
       </c>
       <c r="E1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F1" t="s">
         <v>5</v>
       </c>
       <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
         <v>11</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>12</v>
-      </c>
-      <c r="I1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A2" s="3">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="5">
         <v>42736</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="4">
         <v>10</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="3">
         <v>3</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="3">
         <v>3</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2" s="2">
         <v>100</v>
       </c>
-      <c r="I2" s="4">
+      <c r="I2" s="3">
         <v>65335</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A3" s="3">
+      <c r="A3" s="2">
         <f>1.5</f>
         <v>1.5</v>
       </c>
       <c r="B3" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="5">
         <v>42794</v>
       </c>
       <c r="D3" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="4">
         <v>2.3340000000000001</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="3">
         <v>5</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="3">
         <v>4</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H3" s="2">
         <v>65335</v>
       </c>
-      <c r="I3" s="4">
+      <c r="I3" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A4" s="3">
+      <c r="A4" s="2">
         <v>3.4</v>
       </c>
       <c r="B4" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="5">
         <v>36585</v>
       </c>
       <c r="D4">
         <v>10</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="4">
         <v>4.5</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="3">
         <v>-100</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="3">
         <v>5</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4" s="2">
         <v>1</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4" s="3">
         <v>250</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A5" s="3">
+      <c r="A5" s="2">
         <v>5.5</v>
       </c>
       <c r="B5" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="5">
         <v>42795</v>
       </c>
       <c r="D5" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="4">
         <v>11</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="3">
         <v>2</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="3">
         <v>250</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5" s="2">
         <v>250</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5" s="3">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A6" s="3"/>
+      <c r="A6" s="2"/>
+      <c r="C6" s="5"/>
       <c r="D6" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="4">
         <v>100</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="3">
         <v>3</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="3">
         <v>3</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="2">
         <v>5</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6" s="3">
         <v>3147483647</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A7" s="3">
+      <c r="A7" s="2">
         <v>3.4</v>
       </c>
       <c r="B7" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="5">
         <v>42795</v>
       </c>
       <c r="D7" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="5">
-        <v>2.1</v>
-      </c>
-      <c r="F7" s="4">
+      <c r="E7" s="4">
+        <v>10000.5</v>
+      </c>
+      <c r="F7" s="3">
         <v>120</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="3">
         <v>100</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7" s="2">
         <v>10000</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I7" s="3">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix with respect to write options
</commit_message>
<xml_diff>
--- a/src/it/resources/testsimple.xlsx
+++ b/src/it/resources/testsimple.xlsx
@@ -1,23 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28502"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10309"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/tmp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jornfranke/repos/work/spark-hadoopoffice-ds/src/it/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D251A0CF-84D8-4F44-B637-6B16EE63C933}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19420" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -77,10 +84,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="&quot;WAHR&quot;;&quot;WAHR&quot;;&quot;FALSCH&quot;"/>
-    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -114,17 +121,20 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Stand." xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -392,10 +402,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="96" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>

</xml_diff>